<commit_message>
benchmarks included in main text
</commit_message>
<xml_diff>
--- a/encodingTimeGroupByLargeMem.xlsx
+++ b/encodingTimeGroupByLargeMem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george\Documents\Diplomatiki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE391F37-261B-460D-8DD6-5697916E7EB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D4AFFF-271F-4D9A-B7E1-75D444AFD54D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="0" windowWidth="13845" windowHeight="11385" activeTab="3" xr2:uid="{B15E1454-E382-46F6-BA0B-FABF915355BC}"/>
+    <workbookView xWindow="465" yWindow="15" windowWidth="7500" windowHeight="6000" activeTab="3" xr2:uid="{B15E1454-E382-46F6-BA0B-FABF915355BC}"/>
   </bookViews>
   <sheets>
     <sheet name="uniform" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
   <si>
     <t>RLE</t>
   </si>
@@ -56,26 +56,14 @@
   <si>
     <t>HYBRID_COLUMNAR</t>
   </si>
-  <si>
-    <t>cardinality: 10</t>
-  </si>
-  <si>
-    <t>cardinality: 100</t>
-  </si>
-  <si>
-    <t>cardinality: 1000</t>
-  </si>
-  <si>
-    <t>cardinality: 10000</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -109,8 +97,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -163,7 +151,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Encoding performance per cardinality</a:t>
+              <a:t>Encoding performance [uniform]</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -242,24 +230,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>uniform!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -328,24 +317,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>uniform!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -414,24 +404,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>uniform!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -500,24 +491,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>uniform!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -586,24 +578,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>uniform!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -672,24 +665,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>uniform!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -764,24 +758,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>uniform!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1160,8 +1155,21 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Encoding performance per cardinality</a:t>
+              <a:t>Encoding performance </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="el-GR"/>
+              <a:t>[</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>normal</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="el-GR"/>
+              <a:t>]</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1239,24 +1247,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>normal!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1325,24 +1334,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>normal!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1411,24 +1421,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>normal!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1497,24 +1508,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>normal!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1583,24 +1595,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>normal!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1669,24 +1682,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>normal!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1761,24 +1775,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>normal!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2156,7 +2171,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Encoding performance per cardinality</a:t>
+              <a:t>Encoding performance [exponential 1]</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2235,24 +2250,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 1'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2321,24 +2337,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 1'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2407,24 +2424,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 1'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2493,24 +2511,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 1'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2579,24 +2598,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 1'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2665,24 +2685,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 1'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2757,24 +2778,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 1'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -3152,7 +3174,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Encoding performance per cardinality</a:t>
+              <a:t>Encoding performance [exponential 2]</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3231,24 +3253,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 2'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -3317,24 +3340,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 2'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -3403,24 +3427,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 2'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -3489,24 +3514,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 2'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -3575,24 +3601,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 2'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -3661,24 +3688,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 2'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -3753,24 +3781,25 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>'exponential 2'!$B$1:$E$1</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>cardinality: 10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>cardinality: 100</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>cardinality: 1000</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>cardinality: 10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -6749,7 +6778,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6762,17 +6791,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B1">
         <v>10</v>
+      </c>
+      <c r="C1">
+        <v>100</v>
+      </c>
+      <c r="D1">
+        <v>1000</v>
+      </c>
+      <c r="E1">
+        <v>10000</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6905,7 +6934,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6918,17 +6947,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B1">
         <v>10</v>
+      </c>
+      <c r="C1">
+        <v>100</v>
+      </c>
+      <c r="D1">
+        <v>1000</v>
+      </c>
+      <c r="E1">
+        <v>10000</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -7061,7 +7090,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7074,17 +7103,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B1">
         <v>10</v>
+      </c>
+      <c r="C1">
+        <v>100</v>
+      </c>
+      <c r="D1">
+        <v>1000</v>
+      </c>
+      <c r="E1">
+        <v>10000</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -7217,7 +7246,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7230,17 +7259,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B1">
         <v>10</v>
+      </c>
+      <c r="C1">
+        <v>100</v>
+      </c>
+      <c r="D1">
+        <v>1000</v>
+      </c>
+      <c r="E1">
+        <v>10000</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>